<commit_message>
Changes in the model of the application
</commit_message>
<xml_diff>
--- a/Linked/Principios.xlsx
+++ b/Linked/Principios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante.fit\Desktop\2000ish\2019\UCU\Programacion 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante.fit\Desktop\2000ish\2019\UCU\Programacion 2\pii_2019_equipo1\Linked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106A39A3-9782-42EB-809D-35010FE88FAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67CC879-E384-4920-A73D-0394D9C30F48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{4DF17DAA-7489-40AA-8D08-407845371BB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4DF17DAA-7489-40AA-8D08-407845371BB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -986,7 +986,7 @@
   <dimension ref="B1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="30"/>
       <c r="E23" s="6" t="s">
         <v>21</v>
@@ -1211,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636205C4-AF39-4273-AC98-6321D552655A}">
-  <dimension ref="B1:F6"/>
+  <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>